<commit_message>
changes in home news
</commit_message>
<xml_diff>
--- a/Laravel Learning Log.xlsx
+++ b/Laravel Learning Log.xlsx
@@ -16,22 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>13/7/2017</t>
-  </si>
-  <si>
-    <t>14/7/2017</t>
-  </si>
-  <si>
-    <t>laravel installation</t>
-  </si>
-  <si>
-    <t>template search and local host configuration</t>
-  </si>
-  <si>
-    <t>template porting to laravel</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>DATE</t>
   </si>
@@ -49,13 +34,37 @@
   </si>
   <si>
     <t>:url routing, template inheritance</t>
+  </si>
+  <si>
+    <t>Laravel installation</t>
+  </si>
+  <si>
+    <t>Template search and local host configuration</t>
+  </si>
+  <si>
+    <t>Template porting to laravel</t>
+  </si>
+  <si>
+    <t>Dynamic breaking news creation</t>
+  </si>
+  <si>
+    <t>:eloquent model,fix index.php on laravel,rendering object on view,creating one to many relation, how to loop through related objects</t>
+  </si>
+  <si>
+    <t>Populating sections from the models</t>
+  </si>
+  <si>
+    <t>:eloquent relations, queries in eloquent ordering , creation of multiple views</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+  </numFmts>
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,16 +72,46 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="6" tint="-0.499984740745262"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -80,13 +119,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -384,72 +441,86 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="29.5703125" customWidth="1"/>
-    <col min="2" max="2" width="53.140625" customWidth="1"/>
-    <col min="3" max="3" width="82.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.5703125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="53.140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="82.140625" style="4" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
+    <row r="1" spans="1:3" s="2" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="1">
-        <v>43015</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
+      <c r="A2" s="3">
+        <v>42926</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="1">
-        <v>43046</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
+      <c r="A4" s="3">
+        <v>42927</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="1">
-        <v>43076</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
+      <c r="A6" s="3">
+        <v>42928</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="1" t="s">
-        <v>0</v>
+      <c r="A8" s="3">
+        <v>42929</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="1" t="s">
-        <v>1</v>
+      <c r="A10" s="3">
+        <v>42930</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
changes in magazine app
</commit_message>
<xml_diff>
--- a/Laravel Learning Log.xlsx
+++ b/Laravel Learning Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>DATE</t>
   </si>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t>:using url helpers, fetching slugs from database , more parameters on control functions</t>
+  </si>
+  <si>
+    <t>Angualr JS on Laravel</t>
+  </si>
+  <si>
+    <t>:angular js integration in laravel , integrating the commenting part,recent comments</t>
   </si>
 </sst>
 </file>
@@ -444,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -535,6 +541,17 @@
         <v>14</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="3">
+        <v>42935</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
changes in home news application
</commit_message>
<xml_diff>
--- a/Laravel Learning Log.xlsx
+++ b/Laravel Learning Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>DATE</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>: angular js + kendoui grid , crud functions with laravel</t>
+  </si>
+  <si>
+    <t>Angular routing with kendo grid</t>
+  </si>
+  <si>
+    <t>:separating controllers when routing using angular ngRoutes</t>
   </si>
 </sst>
 </file>
@@ -474,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -618,6 +624,17 @@
       </c>
       <c r="C22" s="4" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="3">
+        <v>42942</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>